<commit_message>
change name for pub dev publish
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\free-mind\games\admin\assets\l10n\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arsen\StudioProjects\arb_excel\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F20AB6-7B54-4111-8AC5-4B22B75E5F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9916C32C-6DE5-4631-9FBB-C3BE5D7B6B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4464" yWindow="1776" windowWidth="15108" windowHeight="12888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Text" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Note" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -229,21 +229,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -251,7 +251,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -259,7 +259,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -267,35 +267,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -303,7 +303,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -311,14 +311,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -326,14 +326,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -341,7 +341,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,14 +349,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -727,50 +727,50 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -786,49 +786,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -872,9 +829,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -912,7 +869,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1018,7 +975,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1160,7 +1117,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1174,16 +1131,16 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1217,7 +1174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1234,7 +1191,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1248,7 +1205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1219,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1273,7 +1230,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1287,7 +1244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1301,7 +1258,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1315,7 +1272,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1286,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1343,7 +1300,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1357,7 +1314,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1371,7 +1328,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1385,7 +1342,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1399,7 +1356,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1413,7 +1370,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1427,7 +1384,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1466,16 +1423,16 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0.8984375" customWidth="1"/>
-    <col min="2" max="2" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>42</v>
       </c>
@@ -1486,12 +1443,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -1500,7 +1457,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>63</v>
       </c>
@@ -1509,7 +1466,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>44</v>
       </c>

</xml_diff>